<commit_message>
Reto 12, resgitar pedido
</commit_message>
<xml_diff>
--- a/Inventario Tablaas.xlsx
+++ b/Inventario Tablaas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Programacion M8\Desktop\Mio\MODULO 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D0FC1D-D630-4B3D-99F9-172F69F61E83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246BCBCA-C805-48F6-96AE-482F38A3DB04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{C09D50AA-B3E7-4138-9155-710AEB92E894}"/>
   </bookViews>
@@ -822,6 +822,7 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -888,7 +889,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1223,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4ED4EDE-1F9F-414E-B947-087CCCD5841E}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="81" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="81" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,17 +1246,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
       <c r="H1" s="2"/>
       <c r="I1" s="51" t="s">
         <v>18</v>
@@ -1467,16 +1467,16 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1615,19 +1615,19 @@
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="68"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="69"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="69" t="s">
+      <c r="H18" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="70"/>
+      <c r="I18" s="71"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
@@ -1708,16 +1708,16 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="D23" s="73" t="s">
+      <c r="B23" s="73"/>
+      <c r="D23" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="76"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="49" t="s">
@@ -1789,14 +1789,14 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="61"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="62"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1888,13 +1888,13 @@
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
@@ -1974,7 +1974,7 @@
       <c r="B40" s="52">
         <v>45605.860439814816</v>
       </c>
-      <c r="C40" s="76" t="s">
+      <c r="C40" s="54" t="s">
         <v>103</v>
       </c>
       <c r="D40" s="25">
@@ -1993,7 +1993,7 @@
       <c r="B41" s="52">
         <v>45605.860439814816</v>
       </c>
-      <c r="C41" s="76" t="s">
+      <c r="C41" s="54" t="s">
         <v>104</v>
       </c>
       <c r="D41" s="25">
@@ -2006,13 +2006,13 @@
       <c r="G41" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
+      <c r="A43" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="56"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="57"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="58"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -2050,15 +2050,15 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="54" t="s">
+      <c r="A47" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="54"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
     </row>
     <row r="48" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
@@ -2087,7 +2087,7 @@
       <c r="A49" s="7">
         <v>1</v>
       </c>
-      <c r="B49" s="76">
+      <c r="B49" s="54">
         <v>1</v>
       </c>
       <c r="C49" s="7">
@@ -2110,7 +2110,7 @@
       <c r="A50" s="7">
         <v>2</v>
       </c>
-      <c r="B50" s="76">
+      <c r="B50" s="54">
         <v>1</v>
       </c>
       <c r="C50" s="7">

</xml_diff>